<commit_message>
add test data file
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -32,65 +32,53 @@
     <t>Test Case Name</t>
   </si>
   <si>
-    <t>aaaa</t>
-  </si>
-  <si>
     <t>testUrl</t>
   </si>
   <si>
-    <t xml:space="preserve">https://recruitingapp-90185108.umantis.com/HiringManager/#/Application/246/508/950 </t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>Gabriela Klein</t>
-  </si>
-  <si>
-    <t>applicant</t>
-  </si>
-  <si>
-    <t>starsNumber</t>
-  </si>
-  <si>
-    <r>
-      <t>Lorem Ipsum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum</t>
-    </r>
-  </si>
-  <si>
-    <t>nextStep</t>
-  </si>
-  <si>
-    <t>Invite for 1st interview</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Wallet@123</t>
   </si>
   <si>
     <t>facebook_test@inbox.ru</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>https://wallethub.com/profile/test_insurance_company/</t>
+  </si>
+  <si>
+    <t>stars_1</t>
+  </si>
+  <si>
+    <t>stars_2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>reviewText</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Aenean commodo ligula eget dolor. Aenean massa. Cum sociis natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Donec qu</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,23 +94,7 @@
       <family val="3"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -146,32 +118,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,78 +424,72 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
     <col min="5" max="7" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="/Application/246/508/950" display="https://recruitingapp-90185108.umantis.com/HiringManager/ - /Application/246/508/950"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
-  <ignoredErrors>
-    <ignoredError sqref="F2" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>